<commit_message>
Finalizada a atualizacao de todos os PADS para o consolidador
</commit_message>
<xml_diff>
--- a/Mapeamento lote 03.xlsx
+++ b/Mapeamento lote 03.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Puc_Lean2016\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15240" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="455.2012" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="3819.2016" sheetId="4" r:id="rId4"/>
     <sheet name="7017.2016" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2124,12 +2119,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2137,6 +2126,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2153,7 +2148,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -14299,9 +14294,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -14339,9 +14334,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14376,7 +14371,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14411,7 +14406,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -14587,7 +14582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18:E48"/>
     </sheetView>
   </sheetViews>
@@ -15314,8 +15309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15327,24 +15322,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>556</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -15356,13 +15351,13 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>265</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -15374,13 +15369,13 @@
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -15392,13 +15387,13 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -16404,15 +16399,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A8:E8"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -16424,8 +16419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F46"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16470,13 +16465,13 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -16491,12 +16486,12 @@
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -16550,13 +16545,13 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -17157,8 +17152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17183,12 +17178,12 @@
       <c r="A2" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>559</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -17200,13 +17195,13 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -17219,12 +17214,12 @@
     </row>
     <row r="6" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -17236,13 +17231,13 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="38" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -18284,8 +18279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18309,12 +18304,12 @@
       <c r="A2" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -18328,13 +18323,13 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>497</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -18349,12 +18344,12 @@
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -18368,13 +18363,13 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="40" t="s">
         <v>499</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>